<commit_message>
Add distribution_seed to test sheets
</commit_message>
<xml_diff>
--- a/tests/fmudesign/data/config/design_input_background.xlsx
+++ b/tests/fmudesign/data/config/design_input_background.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FCUR/git/fmu-tools/tests/sensitivities/data/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LGAZ/semeio/tests/fmudesign/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656DA750-A316-754B-9249-B3C71ED12A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFDEA59-7A10-5944-B771-F473C9BB93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="34600" windowWidth="30240" windowHeight="18880" tabRatio="992" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -55,8 +55,18 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Number of repeated seeds per sensitivity/sensitivity case. 
-This is overrided if number of realisations is specified in the numreal column in designinput.</t>
+          <t xml:space="preserve">Number of repeated seeds per sensitivity/sensitivity case. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This is overrided if number of realisations is specified in the numreal column in designinput.</t>
         </r>
       </text>
     </comment>
@@ -283,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
   <si>
     <t>designtype</t>
   </si>
@@ -523,6 +533,12 @@
   </si>
   <si>
     <t>corr0</t>
+  </si>
+  <si>
+    <t>distribution_seed</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -2696,15 +2712,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.83203125"/>
     <col min="4" max="1025" width="8.6640625"/>
@@ -2740,6 +2756,14 @@
       </c>
       <c r="B4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3597,7 +3621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F3D6AD-89C3-1641-9CBF-9EF76F0F510F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Force distribution seed to be set in user input
Force distribution_seed to be set, either to a number (e.g. 38503) or None. Before, users could avoid setting distribution_seed altogether, which would implicitly set None and make the analysis reproducible. We want to avoid this.
</commit_message>
<xml_diff>
--- a/tests/fmudesign/data/config/design_input_background.xlsx
+++ b/tests/fmudesign/data/config/design_input_background.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FCUR/git/fmu-tools/tests/sensitivities/data/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LGAZ/semeio/tests/fmudesign/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656DA750-A316-754B-9249-B3C71ED12A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFDEA59-7A10-5944-B771-F473C9BB93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="34600" windowWidth="30240" windowHeight="18880" tabRatio="992" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -55,8 +55,18 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Number of repeated seeds per sensitivity/sensitivity case. 
-This is overrided if number of realisations is specified in the numreal column in designinput.</t>
+          <t xml:space="preserve">Number of repeated seeds per sensitivity/sensitivity case. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This is overrided if number of realisations is specified in the numreal column in designinput.</t>
         </r>
       </text>
     </comment>
@@ -283,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
   <si>
     <t>designtype</t>
   </si>
@@ -523,6 +533,12 @@
   </si>
   <si>
     <t>corr0</t>
+  </si>
+  <si>
+    <t>distribution_seed</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -2696,15 +2712,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.83203125"/>
     <col min="4" max="1025" width="8.6640625"/>
@@ -2740,6 +2756,14 @@
       </c>
       <c r="B4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3597,7 +3621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F3D6AD-89C3-1641-9CBF-9EF76F0F510F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update example sheets with new distributions
</commit_message>
<xml_diff>
--- a/tests/fmudesign/data/config/design_input_background.xlsx
+++ b/tests/fmudesign/data/config/design_input_background.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LGAZ/semeio/tests/fmudesign/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFDEA59-7A10-5944-B771-F473C9BB93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330DF5C6-B6E7-8940-A567-F54B2502958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="background" sheetId="5" r:id="rId6"/>
     <sheet name="background_corr" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -177,8 +177,19 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Trine Alsos:
-Distname and dist_param1, .. only for p10_p90 sensitivities or background parameters</t>
+          <t xml:space="preserve">Trine Alsos:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Distname and dist_param1, .. only for p10_p90 sensitivities or background parameters</t>
         </r>
         <r>
           <rPr>
@@ -188,12 +199,62 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Order of distribution parameters must be predefines (and where applicable, same as used for ert in GEN_KW)
-e.g. 
-normal(mean, std dev,min, max) – where min/max is optional and will give truncated gaussian
-lognormal(mean, stddev, min, max) – where min/max is optional and will give truncated lognormal
-uniform(from,to)loguniform(from, to)triangular(low, mode, high)
-discrete((value1, value2, value3,..,value_n) (weight1, weight2, weight3,..weight_n))</t>
+          <t xml:space="preserve">Order of distribution parameters must be predefines (and where applicable, same as used for ert in GEN_KW)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">e.g. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">normal(mean, std dev,min, max) – where min/max is optional and will give truncated gaussian
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">lognormal(mean, stddev, min, max) – where min/max is optional and will give truncated lognormal
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">uniform(from,to)loguniform(from, to)triangular(low, mode, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>discrete((value1, value2, value3,..,value_n) (weight1, weight2, weight3,..weight_n))</t>
         </r>
       </text>
     </comment>
@@ -293,7 +354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="88">
   <si>
     <t>designtype</t>
   </si>
@@ -539,6 +600,24 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>sens9</t>
+  </si>
+  <si>
+    <t>PARAM20</t>
+  </si>
+  <si>
+    <t>normal_p10_p90</t>
+  </si>
+  <si>
+    <t>uniform_p10_p90</t>
+  </si>
+  <si>
+    <t>triangular_p10_p90</t>
+  </si>
+  <si>
+    <t>pert_p10_p90</t>
   </si>
 </sst>
 </file>
@@ -2714,7 +2793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2776,10 +2855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2790,7 +2869,7 @@
     <col min="4" max="4" width="11.83203125"/>
     <col min="5" max="5" width="10" style="2"/>
     <col min="6" max="8" width="11.83203125" style="2"/>
-    <col min="9" max="9" width="11.83203125"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
     <col min="10" max="10" width="33.1640625" style="2"/>
     <col min="11" max="14" width="11.83203125" style="2"/>
     <col min="15" max="17" width="11.83203125"/>
@@ -3377,6 +3456,120 @@
       <c r="N20" s="142"/>
       <c r="O20" s="179"/>
       <c r="P20" s="143"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="132" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="133">
+        <v>500</v>
+      </c>
+      <c r="C21" s="134" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="135" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="176"/>
+      <c r="F21" s="177"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="178"/>
+      <c r="I21" s="138" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="139">
+        <v>0</v>
+      </c>
+      <c r="K21" s="140">
+        <v>1</v>
+      </c>
+      <c r="L21" s="141"/>
+      <c r="M21" s="142"/>
+      <c r="N21" s="142"/>
+      <c r="O21" s="179"/>
+      <c r="P21" s="143"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="132"/>
+      <c r="B22" s="133"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="135" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="176"/>
+      <c r="F22" s="177"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="178"/>
+      <c r="I22" s="138" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" s="139">
+        <v>0.1</v>
+      </c>
+      <c r="K22" s="140">
+        <v>0.9</v>
+      </c>
+      <c r="L22" s="141"/>
+      <c r="M22" s="142"/>
+      <c r="N22" s="142"/>
+      <c r="O22" s="179"/>
+      <c r="P22" s="143"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="132"/>
+      <c r="B23" s="133"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="135" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="176"/>
+      <c r="F23" s="177"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="178"/>
+      <c r="I23" s="138" t="s">
+        <v>86</v>
+      </c>
+      <c r="J23" s="139">
+        <v>0.1</v>
+      </c>
+      <c r="K23" s="140">
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="141">
+        <v>0.9</v>
+      </c>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="179"/>
+      <c r="P23" s="143"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="132"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="135" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="176"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="138" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="139">
+        <v>10</v>
+      </c>
+      <c r="K24" s="140">
+        <v>50</v>
+      </c>
+      <c r="L24" s="141">
+        <v>90</v>
+      </c>
+      <c r="M24" s="142"/>
+      <c r="N24" s="142"/>
+      <c r="O24" s="179"/>
+      <c r="P24" s="143"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add p10 p90 distributions
</commit_message>
<xml_diff>
--- a/tests/fmudesign/data/config/design_input_background.xlsx
+++ b/tests/fmudesign/data/config/design_input_background.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LGAZ/semeio/tests/fmudesign/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFDEA59-7A10-5944-B771-F473C9BB93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598B278F-800E-8342-8F18-05DF97C4C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" tabRatio="992" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="background" sheetId="5" r:id="rId6"/>
     <sheet name="background_corr" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -177,8 +177,19 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Trine Alsos:
-Distname and dist_param1, .. only for p10_p90 sensitivities or background parameters</t>
+          <t xml:space="preserve">Trine Alsos:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Distname and dist_param1, .. only for p10_p90 sensitivities or background parameters</t>
         </r>
         <r>
           <rPr>
@@ -188,12 +199,62 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Order of distribution parameters must be predefines (and where applicable, same as used for ert in GEN_KW)
-e.g. 
-normal(mean, std dev,min, max) – where min/max is optional and will give truncated gaussian
-lognormal(mean, stddev, min, max) – where min/max is optional and will give truncated lognormal
-uniform(from,to)loguniform(from, to)triangular(low, mode, high)
-discrete((value1, value2, value3,..,value_n) (weight1, weight2, weight3,..weight_n))</t>
+          <t xml:space="preserve">Order of distribution parameters must be predefines (and where applicable, same as used for ert in GEN_KW)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">e.g. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">normal(mean, std dev,min, max) – where min/max is optional and will give truncated gaussian
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">lognormal(mean, stddev, min, max) – where min/max is optional and will give truncated lognormal
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">uniform(from,to)loguniform(from, to)triangular(low, mode, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>discrete((value1, value2, value3,..,value_n) (weight1, weight2, weight3,..weight_n))</t>
         </r>
       </text>
     </comment>
@@ -256,8 +317,18 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Used both as default and as base case value for single sensitivities.
-Values can be strings or numbers</t>
+          <t xml:space="preserve">Used both as default and as base case value for single sensitivities.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Values can be strings or numbers</t>
         </r>
       </text>
     </comment>
@@ -293,7 +364,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
   <si>
     <t>designtype</t>
   </si>
@@ -539,6 +610,24 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>sens9</t>
+  </si>
+  <si>
+    <t>PARAM20</t>
+  </si>
+  <si>
+    <t>normal_p10_p90</t>
+  </si>
+  <si>
+    <t>uniform_p10_p90</t>
+  </si>
+  <si>
+    <t>triangular_p10_p90</t>
+  </si>
+  <si>
+    <t>pert_p10_p90</t>
   </si>
 </sst>
 </file>
@@ -2319,7 +2408,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2714,7 +2803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2776,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2790,7 +2879,7 @@
     <col min="4" max="4" width="11.83203125"/>
     <col min="5" max="5" width="10" style="2"/>
     <col min="6" max="8" width="11.83203125" style="2"/>
-    <col min="9" max="9" width="11.83203125"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
     <col min="10" max="10" width="33.1640625" style="2"/>
     <col min="11" max="14" width="11.83203125" style="2"/>
     <col min="15" max="17" width="11.83203125"/>
@@ -3378,6 +3467,120 @@
       <c r="O20" s="179"/>
       <c r="P20" s="143"/>
     </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="132" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="133">
+        <v>500</v>
+      </c>
+      <c r="C21" s="134" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="135" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="176"/>
+      <c r="F21" s="177"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="178"/>
+      <c r="I21" s="138" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="139">
+        <v>0</v>
+      </c>
+      <c r="K21" s="140">
+        <v>1</v>
+      </c>
+      <c r="L21" s="141"/>
+      <c r="M21" s="142"/>
+      <c r="N21" s="142"/>
+      <c r="O21" s="179"/>
+      <c r="P21" s="143"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="132"/>
+      <c r="B22" s="133"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="135" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="176"/>
+      <c r="F22" s="177"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="178"/>
+      <c r="I22" s="138" t="s">
+        <v>84</v>
+      </c>
+      <c r="J22" s="139">
+        <v>0.1</v>
+      </c>
+      <c r="K22" s="140">
+        <v>0.9</v>
+      </c>
+      <c r="L22" s="141"/>
+      <c r="M22" s="142"/>
+      <c r="N22" s="142"/>
+      <c r="O22" s="179"/>
+      <c r="P22" s="143"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="132"/>
+      <c r="B23" s="133"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="135" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="176"/>
+      <c r="F23" s="177"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="178"/>
+      <c r="I23" s="138" t="s">
+        <v>86</v>
+      </c>
+      <c r="J23" s="139">
+        <v>0.1</v>
+      </c>
+      <c r="K23" s="140">
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="141">
+        <v>0.9</v>
+      </c>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="179"/>
+      <c r="P23" s="143"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="132"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="135" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="176"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="138" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="139">
+        <v>10</v>
+      </c>
+      <c r="K24" s="140">
+        <v>50</v>
+      </c>
+      <c r="L24" s="141">
+        <v>90</v>
+      </c>
+      <c r="M24" s="142"/>
+      <c r="N24" s="142"/>
+      <c r="O24" s="179"/>
+      <c r="P24" s="143"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3388,15 +3591,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="2"/>
     <col min="3" max="1025" width="8.6640625"/>
   </cols>
@@ -3582,7 +3785,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3598,7 +3801,7 @@
         <v>73</v>
       </c>
       <c r="B25" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3607,6 +3810,14 @@
       </c>
       <c r="B26" s="2" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>